<commit_message>
Made some changes to Remodel .xlsx. Note: libre edits appeared to remove table from .xoxlsx file
</commit_message>
<xml_diff>
--- a/RemodelPlans.xlsx
+++ b/RemodelPlans.xlsx
@@ -1,107 +1,134 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="539" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="539" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="WholeHouse" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Garage" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="TileRoom" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="MicroRoom" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="FrontRoom" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Kitchen" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Tools" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="WholeHouse" sheetId="1" r:id="rId1"/>
+    <sheet name="Garage" sheetId="2" r:id="rId2"/>
+    <sheet name="TileRoom" sheetId="3" r:id="rId3"/>
+    <sheet name="MicroRoom" sheetId="4" r:id="rId4"/>
+    <sheet name="FrontRoom" sheetId="5" r:id="rId5"/>
+    <sheet name="Kitchen" sheetId="6" r:id="rId6"/>
+    <sheet name="Outside" sheetId="8" r:id="rId7"/>
+    <sheet name="Tools" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Michael.Stanley</author>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A14">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
+          </rPr>
+          <t>Michael.Stanley:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+3/4 vs. 1/2 runs
+types of valves
+list of fittings
+Ground wiring</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Wiring, Plumbing, Lighting Plan done First!
 </t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A15">
+    <comment ref="A15" authorId="1">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Wiring, Plumbing, Lighting Plan done First!
 </t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A16">
+    <comment ref="A16" authorId="1">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Depends on Ceiling replacement method
 </t>
@@ -113,32 +140,32 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Cabinets from Kitchen?
 Shelves from Costco?
@@ -146,29 +173,29 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A4">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
-          <t xml:space="preserve">After Electric</t>
+          <t>After Electric</t>
         </r>
       </text>
     </comment>
@@ -177,58 +204,58 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A5">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
-          <t xml:space="preserve">After Tile is removed</t>
+          <t>After Tile is removed</t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A6">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Decide what we're going to do with them
 Remove/Improve/Keep
@@ -236,27 +263,27 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A7">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">After Ceiling
 After Tile
@@ -265,27 +292,27 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A9">
+    <comment ref="A9" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Mike:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Before: work below floor
 After: Painting/Flooring
@@ -293,27 +320,27 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A16">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Chair rail
 Crown Moulding w/corn.
@@ -328,113 +355,113 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A5">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Temporary Kitchen removal
 </t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A6">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Determine Subfloor Health
 </t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A8">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Relocate Switch. Three Way. 
 </t>
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="A10">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Mold possibility
 </t>
@@ -446,32 +473,32 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A6">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <b val="true"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Kelly:
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
             <charset val="1"/>
-            <family val="2"/>
-            <color rgb="00000000"/>
-            <sz val="9"/>
           </rPr>
           <t xml:space="preserve">Hall Wall. 
 Widen micro room doorway?
@@ -484,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="116">
   <si>
     <t>Description</t>
   </si>
@@ -741,7 +768,7 @@
     <t>Remove Wall?</t>
   </si>
   <si>
-    <t>Redo subfloor </t>
+    <t>Redo subfloor</t>
   </si>
   <si>
     <t>Install rear door?</t>
@@ -783,27 +810,15 @@
     <t>Paint Sprayer</t>
   </si>
   <si>
-    <t>1" screws</t>
-  </si>
-  <si>
     <t>Air compressor</t>
   </si>
   <si>
-    <t>3" Screws</t>
-  </si>
-  <si>
     <t>Nailgun</t>
   </si>
   <si>
-    <t>plywood (shelves)</t>
-  </si>
-  <si>
     <t>Short Ladder</t>
   </si>
   <si>
-    <t>2x4 (shelves)</t>
-  </si>
-  <si>
     <t>Roof ladder</t>
   </si>
   <si>
@@ -822,62 +837,86 @@
     <t>Hedge Trimmer</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Ground wiring</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Harwood flooring nailer</t>
+  </si>
+  <si>
+    <t>Shutters</t>
+  </si>
+  <si>
+    <t>Soffit</t>
+  </si>
+  <si>
+    <t>Pressure wash siding</t>
+  </si>
+  <si>
+    <t>ground cover under deck</t>
+  </si>
+  <si>
+    <t>remove tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
     </font>
     <font>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
     </font>
   </fonts>
   <fills count="2">
@@ -889,7 +928,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -897,82 +936,902 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K32" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+  <autoFilter ref="A3:K32"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Description" dataDxfId="27"/>
+    <tableColumn id="2" name="Category" dataDxfId="26"/>
+    <tableColumn id="3" name="Priority" dataDxfId="25"/>
+    <tableColumn id="4" name="Asset" dataDxfId="24"/>
+    <tableColumn id="5" name="est. Time" dataDxfId="23"/>
+    <tableColumn id="6" name="est. Cost Low" dataDxfId="22"/>
+    <tableColumn id="7" name="est. Cost High" dataDxfId="21"/>
+    <tableColumn id="8" name="Actual Cost" dataDxfId="20"/>
+    <tableColumn id="9" name="Completed" dataDxfId="19"/>
+    <tableColumn id="10" name="Review" dataDxfId="18"/>
+    <tableColumn id="11" name="Column7" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:K25" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="A1:K25"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Description" dataDxfId="14"/>
+    <tableColumn id="2" name="Category" dataDxfId="13"/>
+    <tableColumn id="3" name="Asset" dataDxfId="12"/>
+    <tableColumn id="4" name="Priority" dataDxfId="11"/>
+    <tableColumn id="5" name="est. Time (hrs)" dataDxfId="10"/>
+    <tableColumn id="6" name="est. Cost Low" dataDxfId="9"/>
+    <tableColumn id="7" name="est. Cost High" dataDxfId="8"/>
+    <tableColumn id="8" name="Actual Cost" dataDxfId="7"/>
+    <tableColumn id="9" name="Completed" dataDxfId="6"/>
+    <tableColumn id="10" name="Review" dataDxfId="5"/>
+    <tableColumn id="11" name="Column7" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A4:K26" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A4:K26"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Description"/>
+    <tableColumn id="2" name="Category"/>
+    <tableColumn id="3" name="Priority"/>
+    <tableColumn id="4" name="Asset"/>
+    <tableColumn id="5" name="est. Time (hrs)"/>
+    <tableColumn id="6" name="est. Cost Low"/>
+    <tableColumn id="7" name="est. Cost High"/>
+    <tableColumn id="8" name="Actual Cost"/>
+    <tableColumn id="9" name="Completed"/>
+    <tableColumn id="10" name="Review"/>
+    <tableColumn id="11" name="Column7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A5:K28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A5:K28"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Description"/>
+    <tableColumn id="2" name="Category"/>
+    <tableColumn id="3" name="Priority"/>
+    <tableColumn id="4" name="Asset"/>
+    <tableColumn id="5" name="est. Time (hrs)"/>
+    <tableColumn id="6" name="est. Cost Low"/>
+    <tableColumn id="7" name="est. Cost High"/>
+    <tableColumn id="8" name="Actual Cost"/>
+    <tableColumn id="9" name="Completed"/>
+    <tableColumn id="10" name="Review"/>
+    <tableColumn id="11" name="Column7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A3:N25"/>
+  <dimension ref="A3:AMK32"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.17647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.4745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6196078431373"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.18039215686274"/>
+    <col min="1" max="1" width="22.28515625" style="1"/>
+    <col min="2" max="2" width="16.42578125" style="1"/>
+    <col min="3" max="3" width="11.140625" style="1"/>
+    <col min="4" max="4" width="8.140625" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="16.42578125" style="2"/>
+    <col min="7" max="7" width="16.85546875" style="2"/>
+    <col min="8" max="8" width="14.5703125" style="2"/>
+    <col min="9" max="9" width="13.140625" style="1"/>
+    <col min="10" max="10" width="9.85546875" style="1"/>
+    <col min="11" max="11" width="11.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="12.5703125" style="1"/>
+    <col min="14" max="14" width="13.140625" style="1"/>
+    <col min="15" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3" s="3">
+    <row r="3" spans="1:14" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1017,12 +1876,12 @@
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <v>1000</v>
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1032,11 +1891,11 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1046,11 +1905,11 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <v>800</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1060,14 +1919,14 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1077,14 +1936,14 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <v>1500</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1094,14 +1953,14 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1111,14 +1970,14 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="2">
         <v>300</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1128,11 +1987,11 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="2">
         <v>150</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1142,14 +2001,14 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="2">
         <v>300</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="2">
         <v>600</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +2019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1174,7 +2033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +2047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1198,14 +2057,14 @@
       <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="2">
         <v>500</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1215,10 +2074,10 @@
       <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="2">
         <v>300</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="2">
         <v>1000</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -1228,29 +2087,29 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="2">
         <v>400</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="2">
         <v>1000</v>
       </c>
-      <c r="M18" s="2" t="n">
-        <f aca="false">SUM(F$1:F$1048574)</f>
+      <c r="M18" s="2">
+        <f>SUM(F$1:F$1048574)</f>
         <v>6200</v>
       </c>
-      <c r="N18" s="2" t="n">
-        <f aca="false">SUM(G$1:G$1048574)</f>
+      <c r="N18" s="2">
+        <f>SUM(G$1:G$1048574)</f>
         <v>14750</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1258,7 +2117,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+    <row r="20" spans="1:14">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1268,17 +2127,17 @@
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="6" t="n">
+      <c r="F20" s="6">
         <v>450</v>
       </c>
-      <c r="G20" s="6" t="n">
+      <c r="G20" s="6">
         <v>650</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1286,7 +2145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1294,7 +2153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +2161,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1310,7 +2169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1318,46 +2177,121 @@
         <v>21</v>
       </c>
     </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.0901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.7921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.9098039215686"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.18039215686274"/>
+    <col min="1" max="1" width="21.140625" style="1"/>
+    <col min="2" max="2" width="11.140625" style="1"/>
+    <col min="3" max="3" width="12" style="1"/>
+    <col min="4" max="4" width="14.85546875" style="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1"/>
+    <col min="7" max="7" width="16.85546875" style="1"/>
+    <col min="8" max="8" width="14.5703125" style="1"/>
+    <col min="9" max="9" width="13.140625" style="1"/>
+    <col min="10" max="10" width="9.85546875" style="1"/>
+    <col min="11" max="11" width="11.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="13.85546875" style="1"/>
+    <col min="14" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1" s="3">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1395,20 +2329,20 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>150</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>500</v>
       </c>
       <c r="H2" s="2"/>
@@ -1416,7 +2350,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1426,18 +2360,18 @@
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <v>80</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2">
         <v>250</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -1448,7 +2382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1462,7 +2396,7 @@
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1479,7 +2413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1492,10 +2426,10 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>50</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="2">
         <v>200</v>
       </c>
       <c r="H7" s="2"/>
@@ -1503,7 +2437,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1517,17 +2451,17 @@
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <v>20</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="2">
         <v>200</v>
       </c>
       <c r="H9" s="2"/>
@@ -1535,7 +2469,7 @@
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
@@ -1548,13 +2482,13 @@
       <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="2">
         <v>500</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="2">
         <v>1500</v>
       </c>
       <c r="H10" s="2"/>
@@ -1562,7 +2496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1573,7 +2507,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1584,7 +2518,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
@@ -1596,48 +2530,42 @@
       <c r="H13" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.956862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.7843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.4745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6196078431373"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.9098039215686"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.6352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.18039215686274"/>
+    <col min="1" max="1" width="26" style="1"/>
+    <col min="2" max="2" width="13.85546875" style="1"/>
+    <col min="3" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="16.42578125" style="2"/>
+    <col min="7" max="7" width="16.85546875" style="2"/>
+    <col min="8" max="8" width="14.5703125" style="2"/>
+    <col min="9" max="9" width="13.140625" style="1"/>
+    <col min="10" max="10" width="9.85546875" style="1"/>
+    <col min="11" max="11" width="11.140625" style="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="12.5703125" style="1"/>
+    <col min="14" max="14" width="13.85546875" style="1"/>
+    <col min="15" max="15" width="16.5703125" style="1"/>
+    <col min="16" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1" s="3">
+    <row r="1" spans="1:15" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1675,7 +2603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -1685,17 +2613,17 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>500</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
@@ -1708,20 +2636,20 @@
       <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="1">
         <v>1.5</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
@@ -1734,17 +2662,17 @@
       <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <v>200</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="2">
         <v>400</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -1754,20 +2682,20 @@
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>1.5</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="2">
         <v>30</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -1777,17 +2705,17 @@
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>71</v>
       </c>
@@ -1797,20 +2725,20 @@
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>500</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="2">
         <v>1500</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
@@ -1820,17 +2748,17 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -1840,13 +2768,13 @@
       <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2">
         <v>20</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="2">
         <v>50</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -1856,7 +2784,7 @@
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>75</v>
       </c>
@@ -1866,13 +2794,13 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="1">
         <v>8</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="2">
         <v>80</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="2">
         <v>200</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -1882,7 +2810,7 @@
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -1892,17 +2820,17 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="1">
         <v>16</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="2">
         <v>250</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -1912,17 +2840,17 @@
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="1">
         <v>16</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="2">
         <v>50</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="2">
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -1932,17 +2860,17 @@
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="2">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -1952,13 +2880,13 @@
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="2">
         <v>100</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="2">
         <v>1000</v>
       </c>
       <c r="M14" s="1" t="s">
@@ -1968,7 +2896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -1978,25 +2906,25 @@
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="1">
         <v>4</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="2">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="2">
         <v>100</v>
       </c>
-      <c r="M15" s="2" t="n">
-        <f aca="false">SUM(F$1:F$1048575)</f>
+      <c r="M15" s="2">
+        <f>SUM(F$1:F$1048575)</f>
         <v>1300</v>
       </c>
-      <c r="N15" s="2" t="n">
-        <f aca="false">SUM(G$1:G$1048575)</f>
+      <c r="N15" s="2">
+        <f>SUM(G$1:G$1048575)</f>
         <v>5670</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -2006,17 +2934,17 @@
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="1">
         <v>8</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="2">
         <v>100</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="2">
         <v>600</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>83</v>
       </c>
@@ -2033,44 +2961,37 @@
       <c r="J17" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A4:K11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.956862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
+    <col min="1" max="1" width="26"/>
+    <col min="2" max="2" width="13.85546875"/>
+    <col min="3" max="3" width="11.140625"/>
+    <col min="4" max="4" width="10.28515625"/>
+    <col min="5" max="5" width="16.140625"/>
+    <col min="6" max="6" width="16.42578125"/>
+    <col min="7" max="7" width="16.85546875"/>
+    <col min="8" max="8" width="14.5703125"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="9.85546875"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4" s="3">
+    <row r="4" spans="1:11" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2105,18 +3026,18 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="1">
         <v>16</v>
       </c>
       <c r="F5" s="2"/>
@@ -2126,11 +3047,11 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2144,11 +3065,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2162,11 +3083,11 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2180,14 +3101,14 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="1"/>
@@ -2199,14 +3120,14 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1"/>
@@ -2218,8 +3139,8 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="1"/>
@@ -2233,43 +3154,39 @@
       <c r="K11" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A5:K8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.17647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
+    <col min="1" max="1" width="19.5703125"/>
+    <col min="2" max="3" width="11.140625"/>
+    <col min="4" max="4" width="8.140625"/>
+    <col min="5" max="5" width="16.140625"/>
+    <col min="6" max="6" width="16.42578125"/>
+    <col min="7" max="7" width="16.85546875"/>
+    <col min="8" max="8" width="14.5703125"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="9.85546875"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5" s="3">
+    <row r="5" spans="1:11" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2304,11 +3221,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2323,11 +3240,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2341,18 +3258,18 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2">
         <v>100</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="2">
         <v>600</v>
       </c>
       <c r="H8" s="2"/>
@@ -2361,43 +3278,39 @@
       <c r="K8" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A5:K13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B14" activeCellId="0" pane="topLeft" sqref="B14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.17647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
+    <col min="1" max="1" width="18.140625"/>
+    <col min="2" max="3" width="11.140625"/>
+    <col min="4" max="4" width="8.140625"/>
+    <col min="5" max="5" width="16.140625"/>
+    <col min="6" max="6" width="16.42578125"/>
+    <col min="7" max="7" width="16.85546875"/>
+    <col min="8" max="8" width="14.5703125"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="9.85546875"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2432,11 +3345,11 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2451,11 +3364,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2469,11 +3382,11 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2487,11 +3400,11 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2505,14 +3418,14 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="1"/>
@@ -2524,14 +3437,14 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="1"/>
@@ -2543,11 +3456,11 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2562,24 +3475,24 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="2">
         <v>50</v>
       </c>
       <c r="H13" s="2"/>
@@ -2588,42 +3501,132 @@
       <c r="K13" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A3:K11"/>
+  <dimension ref="A4:K10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.140625"/>
+    <col min="4" max="4" width="8.140625"/>
+    <col min="5" max="5" width="16.140625"/>
+    <col min="6" max="6" width="16.42578125"/>
+    <col min="7" max="7" width="16.85546875"/>
+    <col min="8" max="8" width="14.5703125"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="9.85546875"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:K12"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375"/>
+    <col min="2" max="3" width="11.140625"/>
+    <col min="4" max="4" width="24.140625"/>
+    <col min="5" max="5" width="16.140625"/>
+    <col min="6" max="6" width="16.42578125"/>
+    <col min="7" max="7" width="16.85546875"/>
+    <col min="8" max="8" width="14.5703125"/>
+    <col min="9" max="9" width="13.140625"/>
+    <col min="10" max="10" width="9.85546875"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="1025" width="8.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>96</v>
       </c>
@@ -2631,22 +3634,22 @@
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="0" t="s">
-        <v>101</v>
+      <c r="D5" t="s">
+        <v>105</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2655,14 +3658,11 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
-        <v>102</v>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>100</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="7"/>
@@ -2671,14 +3671,11 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
-        <v>104</v>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>101</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2687,14 +3684,11 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
-        <v>106</v>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2703,14 +3697,11 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
-        <v>108</v>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>104</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2719,9 +3710,9 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
-        <v>110</v>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>106</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2732,9 +3723,9 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
-        <v>111</v>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>107</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2745,84 +3736,13 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A4:K4"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.17647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.89411764705882"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.56862745098039"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some files and made some changes
</commit_message>
<xml_diff>
--- a/RemodelPlans.xlsx
+++ b/RemodelPlans.xlsx
@@ -951,7 +951,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -968,6 +968,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1024,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1048,11 +1054,22 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1127,13 +1144,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1145,37 +1155,14 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.59999389629810485"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1433,7 +1420,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1449,6 +1436,13 @@
       </font>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1460,10 +1454,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2216,6 +2226,300 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="shapetype_75" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 9" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 8" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2335,6 +2639,202 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2052" name="AutoShape 4" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="shapetype_75" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 4" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2912,6 +3412,496 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="shapetype_75" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 13" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 12" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 11" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 10" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3227,6 +4217,398 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4104" name="AutoShape 8" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="shapetype_75" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 10" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 9" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 8" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3412,6 +4794,104 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="shapetype_75" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="G0" fmla="+- 2700 0 0"/>
+            <a:gd name="G1" fmla="+- 21600 0 G0"/>
+            <a:gd name="G2" fmla="+- 21600 0 G0"/>
+            <a:gd name="T0" fmla="*/ G0 w 21600"/>
+            <a:gd name="T1" fmla="*/ G0 h 21600"/>
+            <a:gd name="T2" fmla="*/ G1 w 21600"/>
+            <a:gd name="T3" fmla="*/ G2 h 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="r" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="5400000">
+              <a:pos x="hc" y="b"/>
+            </a:cxn>
+            <a:cxn ang="10800000">
+              <a:pos x="l" y="vc"/>
+            </a:cxn>
+            <a:cxn ang="16200000">
+              <a:pos x="hc" y="t"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="T0" t="T1" r="T2" b="T3"/>
+          <a:pathLst>
+            <a:path w="21600" h="21600">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="21600" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="21600" y="21600"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="21600"/>
+              </a:lnTo>
+              <a:close/>
+              <a:moveTo>
+                <a:pt x="2700" y="2700"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="2700" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="18900"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="18900" y="2700"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3456,30 +4936,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:N20" totalsRowShown="0" headerRowDxfId="4" dataDxfId="6" headerRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:N20" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21">
   <autoFilter ref="A1:N20"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Description" dataDxfId="20"/>
-    <tableColumn id="2" name="Category" dataDxfId="19"/>
-    <tableColumn id="3" name="Priority" dataDxfId="18"/>
-    <tableColumn id="4" name="Asset" dataDxfId="17"/>
-    <tableColumn id="5" name="est. Time (hrs)" dataDxfId="16"/>
-    <tableColumn id="6" name="est. Cost Low" dataDxfId="15"/>
-    <tableColumn id="7" name="est. Cost High" dataDxfId="14"/>
-    <tableColumn id="8" name="Actual Cost" dataDxfId="13"/>
-    <tableColumn id="9" name="Completed" dataDxfId="12"/>
-    <tableColumn id="10" name="Review" dataDxfId="11"/>
-    <tableColumn id="11" name="Column7" dataDxfId="10"/>
-    <tableColumn id="12" name="Column8" dataDxfId="9"/>
-    <tableColumn id="13" name="Column9" dataDxfId="8"/>
-    <tableColumn id="14" name="Categories" dataDxfId="7"/>
+    <tableColumn id="1" name="Description" dataDxfId="19"/>
+    <tableColumn id="2" name="Category" dataDxfId="18"/>
+    <tableColumn id="3" name="Priority" dataDxfId="17"/>
+    <tableColumn id="4" name="Asset" dataDxfId="16"/>
+    <tableColumn id="5" name="est. Time (hrs)" dataDxfId="15"/>
+    <tableColumn id="6" name="est. Cost Low" dataDxfId="14"/>
+    <tableColumn id="7" name="est. Cost High" dataDxfId="13"/>
+    <tableColumn id="8" name="Actual Cost" dataDxfId="12"/>
+    <tableColumn id="9" name="Completed" dataDxfId="11"/>
+    <tableColumn id="10" name="Review" dataDxfId="10"/>
+    <tableColumn id="11" name="Column7" dataDxfId="9"/>
+    <tableColumn id="12" name="Column8" dataDxfId="8"/>
+    <tableColumn id="13" name="Column9" dataDxfId="7"/>
+    <tableColumn id="14" name="Categories" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:K23" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:K23" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:K23"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Description"/>
@@ -3499,7 +4979,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:K24" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:K24" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:K24"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Description"/>
@@ -3519,7 +4999,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K14" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:K14" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
   <autoFilter ref="A1:K14"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Description"/>
@@ -3539,7 +5019,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:K9" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <autoFilter ref="A1:K9"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Description"/>
@@ -3847,7 +5327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AMK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -4608,7 +6088,7 @@
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,23 +6483,1038 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:1025" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="25"/>
+      <c r="AD17" s="25"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AJ17" s="25"/>
+      <c r="AK17" s="25"/>
+      <c r="AL17" s="25"/>
+      <c r="AM17" s="25"/>
+      <c r="AN17" s="25"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
+      <c r="AQ17" s="25"/>
+      <c r="AR17" s="25"/>
+      <c r="AS17" s="25"/>
+      <c r="AT17" s="25"/>
+      <c r="AU17" s="25"/>
+      <c r="AV17" s="25"/>
+      <c r="AW17" s="25"/>
+      <c r="AX17" s="25"/>
+      <c r="AY17" s="25"/>
+      <c r="AZ17" s="25"/>
+      <c r="BA17" s="25"/>
+      <c r="BB17" s="25"/>
+      <c r="BC17" s="25"/>
+      <c r="BD17" s="25"/>
+      <c r="BE17" s="25"/>
+      <c r="BF17" s="25"/>
+      <c r="BG17" s="25"/>
+      <c r="BH17" s="25"/>
+      <c r="BI17" s="25"/>
+      <c r="BJ17" s="25"/>
+      <c r="BK17" s="25"/>
+      <c r="BL17" s="25"/>
+      <c r="BM17" s="25"/>
+      <c r="BN17" s="25"/>
+      <c r="BO17" s="25"/>
+      <c r="BP17" s="25"/>
+      <c r="BQ17" s="25"/>
+      <c r="BR17" s="25"/>
+      <c r="BS17" s="25"/>
+      <c r="BT17" s="25"/>
+      <c r="BU17" s="25"/>
+      <c r="BV17" s="25"/>
+      <c r="BW17" s="25"/>
+      <c r="BX17" s="25"/>
+      <c r="BY17" s="25"/>
+      <c r="BZ17" s="25"/>
+      <c r="CA17" s="25"/>
+      <c r="CB17" s="25"/>
+      <c r="CC17" s="25"/>
+      <c r="CD17" s="25"/>
+      <c r="CE17" s="25"/>
+      <c r="CF17" s="25"/>
+      <c r="CG17" s="25"/>
+      <c r="CH17" s="25"/>
+      <c r="CI17" s="25"/>
+      <c r="CJ17" s="25"/>
+      <c r="CK17" s="25"/>
+      <c r="CL17" s="25"/>
+      <c r="CM17" s="25"/>
+      <c r="CN17" s="25"/>
+      <c r="CO17" s="25"/>
+      <c r="CP17" s="25"/>
+      <c r="CQ17" s="25"/>
+      <c r="CR17" s="25"/>
+      <c r="CS17" s="25"/>
+      <c r="CT17" s="25"/>
+      <c r="CU17" s="25"/>
+      <c r="CV17" s="25"/>
+      <c r="CW17" s="25"/>
+      <c r="CX17" s="25"/>
+      <c r="CY17" s="25"/>
+      <c r="CZ17" s="25"/>
+      <c r="DA17" s="25"/>
+      <c r="DB17" s="25"/>
+      <c r="DC17" s="25"/>
+      <c r="DD17" s="25"/>
+      <c r="DE17" s="25"/>
+      <c r="DF17" s="25"/>
+      <c r="DG17" s="25"/>
+      <c r="DH17" s="25"/>
+      <c r="DI17" s="25"/>
+      <c r="DJ17" s="25"/>
+      <c r="DK17" s="25"/>
+      <c r="DL17" s="25"/>
+      <c r="DM17" s="25"/>
+      <c r="DN17" s="25"/>
+      <c r="DO17" s="25"/>
+      <c r="DP17" s="25"/>
+      <c r="DQ17" s="25"/>
+      <c r="DR17" s="25"/>
+      <c r="DS17" s="25"/>
+      <c r="DT17" s="25"/>
+      <c r="DU17" s="25"/>
+      <c r="DV17" s="25"/>
+      <c r="DW17" s="25"/>
+      <c r="DX17" s="25"/>
+      <c r="DY17" s="25"/>
+      <c r="DZ17" s="25"/>
+      <c r="EA17" s="25"/>
+      <c r="EB17" s="25"/>
+      <c r="EC17" s="25"/>
+      <c r="ED17" s="25"/>
+      <c r="EE17" s="25"/>
+      <c r="EF17" s="25"/>
+      <c r="EG17" s="25"/>
+      <c r="EH17" s="25"/>
+      <c r="EI17" s="25"/>
+      <c r="EJ17" s="25"/>
+      <c r="EK17" s="25"/>
+      <c r="EL17" s="25"/>
+      <c r="EM17" s="25"/>
+      <c r="EN17" s="25"/>
+      <c r="EO17" s="25"/>
+      <c r="EP17" s="25"/>
+      <c r="EQ17" s="25"/>
+      <c r="ER17" s="25"/>
+      <c r="ES17" s="25"/>
+      <c r="ET17" s="25"/>
+      <c r="EU17" s="25"/>
+      <c r="EV17" s="25"/>
+      <c r="EW17" s="25"/>
+      <c r="EX17" s="25"/>
+      <c r="EY17" s="25"/>
+      <c r="EZ17" s="25"/>
+      <c r="FA17" s="25"/>
+      <c r="FB17" s="25"/>
+      <c r="FC17" s="25"/>
+      <c r="FD17" s="25"/>
+      <c r="FE17" s="25"/>
+      <c r="FF17" s="25"/>
+      <c r="FG17" s="25"/>
+      <c r="FH17" s="25"/>
+      <c r="FI17" s="25"/>
+      <c r="FJ17" s="25"/>
+      <c r="FK17" s="25"/>
+      <c r="FL17" s="25"/>
+      <c r="FM17" s="25"/>
+      <c r="FN17" s="25"/>
+      <c r="FO17" s="25"/>
+      <c r="FP17" s="25"/>
+      <c r="FQ17" s="25"/>
+      <c r="FR17" s="25"/>
+      <c r="FS17" s="25"/>
+      <c r="FT17" s="25"/>
+      <c r="FU17" s="25"/>
+      <c r="FV17" s="25"/>
+      <c r="FW17" s="25"/>
+      <c r="FX17" s="25"/>
+      <c r="FY17" s="25"/>
+      <c r="FZ17" s="25"/>
+      <c r="GA17" s="25"/>
+      <c r="GB17" s="25"/>
+      <c r="GC17" s="25"/>
+      <c r="GD17" s="25"/>
+      <c r="GE17" s="25"/>
+      <c r="GF17" s="25"/>
+      <c r="GG17" s="25"/>
+      <c r="GH17" s="25"/>
+      <c r="GI17" s="25"/>
+      <c r="GJ17" s="25"/>
+      <c r="GK17" s="25"/>
+      <c r="GL17" s="25"/>
+      <c r="GM17" s="25"/>
+      <c r="GN17" s="25"/>
+      <c r="GO17" s="25"/>
+      <c r="GP17" s="25"/>
+      <c r="GQ17" s="25"/>
+      <c r="GR17" s="25"/>
+      <c r="GS17" s="25"/>
+      <c r="GT17" s="25"/>
+      <c r="GU17" s="25"/>
+      <c r="GV17" s="25"/>
+      <c r="GW17" s="25"/>
+      <c r="GX17" s="25"/>
+      <c r="GY17" s="25"/>
+      <c r="GZ17" s="25"/>
+      <c r="HA17" s="25"/>
+      <c r="HB17" s="25"/>
+      <c r="HC17" s="25"/>
+      <c r="HD17" s="25"/>
+      <c r="HE17" s="25"/>
+      <c r="HF17" s="25"/>
+      <c r="HG17" s="25"/>
+      <c r="HH17" s="25"/>
+      <c r="HI17" s="25"/>
+      <c r="HJ17" s="25"/>
+      <c r="HK17" s="25"/>
+      <c r="HL17" s="25"/>
+      <c r="HM17" s="25"/>
+      <c r="HN17" s="25"/>
+      <c r="HO17" s="25"/>
+      <c r="HP17" s="25"/>
+      <c r="HQ17" s="25"/>
+      <c r="HR17" s="25"/>
+      <c r="HS17" s="25"/>
+      <c r="HT17" s="25"/>
+      <c r="HU17" s="25"/>
+      <c r="HV17" s="25"/>
+      <c r="HW17" s="25"/>
+      <c r="HX17" s="25"/>
+      <c r="HY17" s="25"/>
+      <c r="HZ17" s="25"/>
+      <c r="IA17" s="25"/>
+      <c r="IB17" s="25"/>
+      <c r="IC17" s="25"/>
+      <c r="ID17" s="25"/>
+      <c r="IE17" s="25"/>
+      <c r="IF17" s="25"/>
+      <c r="IG17" s="25"/>
+      <c r="IH17" s="25"/>
+      <c r="II17" s="25"/>
+      <c r="IJ17" s="25"/>
+      <c r="IK17" s="25"/>
+      <c r="IL17" s="25"/>
+      <c r="IM17" s="25"/>
+      <c r="IN17" s="25"/>
+      <c r="IO17" s="25"/>
+      <c r="IP17" s="25"/>
+      <c r="IQ17" s="25"/>
+      <c r="IR17" s="25"/>
+      <c r="IS17" s="25"/>
+      <c r="IT17" s="25"/>
+      <c r="IU17" s="25"/>
+      <c r="IV17" s="25"/>
+      <c r="IW17" s="25"/>
+      <c r="IX17" s="25"/>
+      <c r="IY17" s="25"/>
+      <c r="IZ17" s="25"/>
+      <c r="JA17" s="25"/>
+      <c r="JB17" s="25"/>
+      <c r="JC17" s="25"/>
+      <c r="JD17" s="25"/>
+      <c r="JE17" s="25"/>
+      <c r="JF17" s="25"/>
+      <c r="JG17" s="25"/>
+      <c r="JH17" s="25"/>
+      <c r="JI17" s="25"/>
+      <c r="JJ17" s="25"/>
+      <c r="JK17" s="25"/>
+      <c r="JL17" s="25"/>
+      <c r="JM17" s="25"/>
+      <c r="JN17" s="25"/>
+      <c r="JO17" s="25"/>
+      <c r="JP17" s="25"/>
+      <c r="JQ17" s="25"/>
+      <c r="JR17" s="25"/>
+      <c r="JS17" s="25"/>
+      <c r="JT17" s="25"/>
+      <c r="JU17" s="25"/>
+      <c r="JV17" s="25"/>
+      <c r="JW17" s="25"/>
+      <c r="JX17" s="25"/>
+      <c r="JY17" s="25"/>
+      <c r="JZ17" s="25"/>
+      <c r="KA17" s="25"/>
+      <c r="KB17" s="25"/>
+      <c r="KC17" s="25"/>
+      <c r="KD17" s="25"/>
+      <c r="KE17" s="25"/>
+      <c r="KF17" s="25"/>
+      <c r="KG17" s="25"/>
+      <c r="KH17" s="25"/>
+      <c r="KI17" s="25"/>
+      <c r="KJ17" s="25"/>
+      <c r="KK17" s="25"/>
+      <c r="KL17" s="25"/>
+      <c r="KM17" s="25"/>
+      <c r="KN17" s="25"/>
+      <c r="KO17" s="25"/>
+      <c r="KP17" s="25"/>
+      <c r="KQ17" s="25"/>
+      <c r="KR17" s="25"/>
+      <c r="KS17" s="25"/>
+      <c r="KT17" s="25"/>
+      <c r="KU17" s="25"/>
+      <c r="KV17" s="25"/>
+      <c r="KW17" s="25"/>
+      <c r="KX17" s="25"/>
+      <c r="KY17" s="25"/>
+      <c r="KZ17" s="25"/>
+      <c r="LA17" s="25"/>
+      <c r="LB17" s="25"/>
+      <c r="LC17" s="25"/>
+      <c r="LD17" s="25"/>
+      <c r="LE17" s="25"/>
+      <c r="LF17" s="25"/>
+      <c r="LG17" s="25"/>
+      <c r="LH17" s="25"/>
+      <c r="LI17" s="25"/>
+      <c r="LJ17" s="25"/>
+      <c r="LK17" s="25"/>
+      <c r="LL17" s="25"/>
+      <c r="LM17" s="25"/>
+      <c r="LN17" s="25"/>
+      <c r="LO17" s="25"/>
+      <c r="LP17" s="25"/>
+      <c r="LQ17" s="25"/>
+      <c r="LR17" s="25"/>
+      <c r="LS17" s="25"/>
+      <c r="LT17" s="25"/>
+      <c r="LU17" s="25"/>
+      <c r="LV17" s="25"/>
+      <c r="LW17" s="25"/>
+      <c r="LX17" s="25"/>
+      <c r="LY17" s="25"/>
+      <c r="LZ17" s="25"/>
+      <c r="MA17" s="25"/>
+      <c r="MB17" s="25"/>
+      <c r="MC17" s="25"/>
+      <c r="MD17" s="25"/>
+      <c r="ME17" s="25"/>
+      <c r="MF17" s="25"/>
+      <c r="MG17" s="25"/>
+      <c r="MH17" s="25"/>
+      <c r="MI17" s="25"/>
+      <c r="MJ17" s="25"/>
+      <c r="MK17" s="25"/>
+      <c r="ML17" s="25"/>
+      <c r="MM17" s="25"/>
+      <c r="MN17" s="25"/>
+      <c r="MO17" s="25"/>
+      <c r="MP17" s="25"/>
+      <c r="MQ17" s="25"/>
+      <c r="MR17" s="25"/>
+      <c r="MS17" s="25"/>
+      <c r="MT17" s="25"/>
+      <c r="MU17" s="25"/>
+      <c r="MV17" s="25"/>
+      <c r="MW17" s="25"/>
+      <c r="MX17" s="25"/>
+      <c r="MY17" s="25"/>
+      <c r="MZ17" s="25"/>
+      <c r="NA17" s="25"/>
+      <c r="NB17" s="25"/>
+      <c r="NC17" s="25"/>
+      <c r="ND17" s="25"/>
+      <c r="NE17" s="25"/>
+      <c r="NF17" s="25"/>
+      <c r="NG17" s="25"/>
+      <c r="NH17" s="25"/>
+      <c r="NI17" s="25"/>
+      <c r="NJ17" s="25"/>
+      <c r="NK17" s="25"/>
+      <c r="NL17" s="25"/>
+      <c r="NM17" s="25"/>
+      <c r="NN17" s="25"/>
+      <c r="NO17" s="25"/>
+      <c r="NP17" s="25"/>
+      <c r="NQ17" s="25"/>
+      <c r="NR17" s="25"/>
+      <c r="NS17" s="25"/>
+      <c r="NT17" s="25"/>
+      <c r="NU17" s="25"/>
+      <c r="NV17" s="25"/>
+      <c r="NW17" s="25"/>
+      <c r="NX17" s="25"/>
+      <c r="NY17" s="25"/>
+      <c r="NZ17" s="25"/>
+      <c r="OA17" s="25"/>
+      <c r="OB17" s="25"/>
+      <c r="OC17" s="25"/>
+      <c r="OD17" s="25"/>
+      <c r="OE17" s="25"/>
+      <c r="OF17" s="25"/>
+      <c r="OG17" s="25"/>
+      <c r="OH17" s="25"/>
+      <c r="OI17" s="25"/>
+      <c r="OJ17" s="25"/>
+      <c r="OK17" s="25"/>
+      <c r="OL17" s="25"/>
+      <c r="OM17" s="25"/>
+      <c r="ON17" s="25"/>
+      <c r="OO17" s="25"/>
+      <c r="OP17" s="25"/>
+      <c r="OQ17" s="25"/>
+      <c r="OR17" s="25"/>
+      <c r="OS17" s="25"/>
+      <c r="OT17" s="25"/>
+      <c r="OU17" s="25"/>
+      <c r="OV17" s="25"/>
+      <c r="OW17" s="25"/>
+      <c r="OX17" s="25"/>
+      <c r="OY17" s="25"/>
+      <c r="OZ17" s="25"/>
+      <c r="PA17" s="25"/>
+      <c r="PB17" s="25"/>
+      <c r="PC17" s="25"/>
+      <c r="PD17" s="25"/>
+      <c r="PE17" s="25"/>
+      <c r="PF17" s="25"/>
+      <c r="PG17" s="25"/>
+      <c r="PH17" s="25"/>
+      <c r="PI17" s="25"/>
+      <c r="PJ17" s="25"/>
+      <c r="PK17" s="25"/>
+      <c r="PL17" s="25"/>
+      <c r="PM17" s="25"/>
+      <c r="PN17" s="25"/>
+      <c r="PO17" s="25"/>
+      <c r="PP17" s="25"/>
+      <c r="PQ17" s="25"/>
+      <c r="PR17" s="25"/>
+      <c r="PS17" s="25"/>
+      <c r="PT17" s="25"/>
+      <c r="PU17" s="25"/>
+      <c r="PV17" s="25"/>
+      <c r="PW17" s="25"/>
+      <c r="PX17" s="25"/>
+      <c r="PY17" s="25"/>
+      <c r="PZ17" s="25"/>
+      <c r="QA17" s="25"/>
+      <c r="QB17" s="25"/>
+      <c r="QC17" s="25"/>
+      <c r="QD17" s="25"/>
+      <c r="QE17" s="25"/>
+      <c r="QF17" s="25"/>
+      <c r="QG17" s="25"/>
+      <c r="QH17" s="25"/>
+      <c r="QI17" s="25"/>
+      <c r="QJ17" s="25"/>
+      <c r="QK17" s="25"/>
+      <c r="QL17" s="25"/>
+      <c r="QM17" s="25"/>
+      <c r="QN17" s="25"/>
+      <c r="QO17" s="25"/>
+      <c r="QP17" s="25"/>
+      <c r="QQ17" s="25"/>
+      <c r="QR17" s="25"/>
+      <c r="QS17" s="25"/>
+      <c r="QT17" s="25"/>
+      <c r="QU17" s="25"/>
+      <c r="QV17" s="25"/>
+      <c r="QW17" s="25"/>
+      <c r="QX17" s="25"/>
+      <c r="QY17" s="25"/>
+      <c r="QZ17" s="25"/>
+      <c r="RA17" s="25"/>
+      <c r="RB17" s="25"/>
+      <c r="RC17" s="25"/>
+      <c r="RD17" s="25"/>
+      <c r="RE17" s="25"/>
+      <c r="RF17" s="25"/>
+      <c r="RG17" s="25"/>
+      <c r="RH17" s="25"/>
+      <c r="RI17" s="25"/>
+      <c r="RJ17" s="25"/>
+      <c r="RK17" s="25"/>
+      <c r="RL17" s="25"/>
+      <c r="RM17" s="25"/>
+      <c r="RN17" s="25"/>
+      <c r="RO17" s="25"/>
+      <c r="RP17" s="25"/>
+      <c r="RQ17" s="25"/>
+      <c r="RR17" s="25"/>
+      <c r="RS17" s="25"/>
+      <c r="RT17" s="25"/>
+      <c r="RU17" s="25"/>
+      <c r="RV17" s="25"/>
+      <c r="RW17" s="25"/>
+      <c r="RX17" s="25"/>
+      <c r="RY17" s="25"/>
+      <c r="RZ17" s="25"/>
+      <c r="SA17" s="25"/>
+      <c r="SB17" s="25"/>
+      <c r="SC17" s="25"/>
+      <c r="SD17" s="25"/>
+      <c r="SE17" s="25"/>
+      <c r="SF17" s="25"/>
+      <c r="SG17" s="25"/>
+      <c r="SH17" s="25"/>
+      <c r="SI17" s="25"/>
+      <c r="SJ17" s="25"/>
+      <c r="SK17" s="25"/>
+      <c r="SL17" s="25"/>
+      <c r="SM17" s="25"/>
+      <c r="SN17" s="25"/>
+      <c r="SO17" s="25"/>
+      <c r="SP17" s="25"/>
+      <c r="SQ17" s="25"/>
+      <c r="SR17" s="25"/>
+      <c r="SS17" s="25"/>
+      <c r="ST17" s="25"/>
+      <c r="SU17" s="25"/>
+      <c r="SV17" s="25"/>
+      <c r="SW17" s="25"/>
+      <c r="SX17" s="25"/>
+      <c r="SY17" s="25"/>
+      <c r="SZ17" s="25"/>
+      <c r="TA17" s="25"/>
+      <c r="TB17" s="25"/>
+      <c r="TC17" s="25"/>
+      <c r="TD17" s="25"/>
+      <c r="TE17" s="25"/>
+      <c r="TF17" s="25"/>
+      <c r="TG17" s="25"/>
+      <c r="TH17" s="25"/>
+      <c r="TI17" s="25"/>
+      <c r="TJ17" s="25"/>
+      <c r="TK17" s="25"/>
+      <c r="TL17" s="25"/>
+      <c r="TM17" s="25"/>
+      <c r="TN17" s="25"/>
+      <c r="TO17" s="25"/>
+      <c r="TP17" s="25"/>
+      <c r="TQ17" s="25"/>
+      <c r="TR17" s="25"/>
+      <c r="TS17" s="25"/>
+      <c r="TT17" s="25"/>
+      <c r="TU17" s="25"/>
+      <c r="TV17" s="25"/>
+      <c r="TW17" s="25"/>
+      <c r="TX17" s="25"/>
+      <c r="TY17" s="25"/>
+      <c r="TZ17" s="25"/>
+      <c r="UA17" s="25"/>
+      <c r="UB17" s="25"/>
+      <c r="UC17" s="25"/>
+      <c r="UD17" s="25"/>
+      <c r="UE17" s="25"/>
+      <c r="UF17" s="25"/>
+      <c r="UG17" s="25"/>
+      <c r="UH17" s="25"/>
+      <c r="UI17" s="25"/>
+      <c r="UJ17" s="25"/>
+      <c r="UK17" s="25"/>
+      <c r="UL17" s="25"/>
+      <c r="UM17" s="25"/>
+      <c r="UN17" s="25"/>
+      <c r="UO17" s="25"/>
+      <c r="UP17" s="25"/>
+      <c r="UQ17" s="25"/>
+      <c r="UR17" s="25"/>
+      <c r="US17" s="25"/>
+      <c r="UT17" s="25"/>
+      <c r="UU17" s="25"/>
+      <c r="UV17" s="25"/>
+      <c r="UW17" s="25"/>
+      <c r="UX17" s="25"/>
+      <c r="UY17" s="25"/>
+      <c r="UZ17" s="25"/>
+      <c r="VA17" s="25"/>
+      <c r="VB17" s="25"/>
+      <c r="VC17" s="25"/>
+      <c r="VD17" s="25"/>
+      <c r="VE17" s="25"/>
+      <c r="VF17" s="25"/>
+      <c r="VG17" s="25"/>
+      <c r="VH17" s="25"/>
+      <c r="VI17" s="25"/>
+      <c r="VJ17" s="25"/>
+      <c r="VK17" s="25"/>
+      <c r="VL17" s="25"/>
+      <c r="VM17" s="25"/>
+      <c r="VN17" s="25"/>
+      <c r="VO17" s="25"/>
+      <c r="VP17" s="25"/>
+      <c r="VQ17" s="25"/>
+      <c r="VR17" s="25"/>
+      <c r="VS17" s="25"/>
+      <c r="VT17" s="25"/>
+      <c r="VU17" s="25"/>
+      <c r="VV17" s="25"/>
+      <c r="VW17" s="25"/>
+      <c r="VX17" s="25"/>
+      <c r="VY17" s="25"/>
+      <c r="VZ17" s="25"/>
+      <c r="WA17" s="25"/>
+      <c r="WB17" s="25"/>
+      <c r="WC17" s="25"/>
+      <c r="WD17" s="25"/>
+      <c r="WE17" s="25"/>
+      <c r="WF17" s="25"/>
+      <c r="WG17" s="25"/>
+      <c r="WH17" s="25"/>
+      <c r="WI17" s="25"/>
+      <c r="WJ17" s="25"/>
+      <c r="WK17" s="25"/>
+      <c r="WL17" s="25"/>
+      <c r="WM17" s="25"/>
+      <c r="WN17" s="25"/>
+      <c r="WO17" s="25"/>
+      <c r="WP17" s="25"/>
+      <c r="WQ17" s="25"/>
+      <c r="WR17" s="25"/>
+      <c r="WS17" s="25"/>
+      <c r="WT17" s="25"/>
+      <c r="WU17" s="25"/>
+      <c r="WV17" s="25"/>
+      <c r="WW17" s="25"/>
+      <c r="WX17" s="25"/>
+      <c r="WY17" s="25"/>
+      <c r="WZ17" s="25"/>
+      <c r="XA17" s="25"/>
+      <c r="XB17" s="25"/>
+      <c r="XC17" s="25"/>
+      <c r="XD17" s="25"/>
+      <c r="XE17" s="25"/>
+      <c r="XF17" s="25"/>
+      <c r="XG17" s="25"/>
+      <c r="XH17" s="25"/>
+      <c r="XI17" s="25"/>
+      <c r="XJ17" s="25"/>
+      <c r="XK17" s="25"/>
+      <c r="XL17" s="25"/>
+      <c r="XM17" s="25"/>
+      <c r="XN17" s="25"/>
+      <c r="XO17" s="25"/>
+      <c r="XP17" s="25"/>
+      <c r="XQ17" s="25"/>
+      <c r="XR17" s="25"/>
+      <c r="XS17" s="25"/>
+      <c r="XT17" s="25"/>
+      <c r="XU17" s="25"/>
+      <c r="XV17" s="25"/>
+      <c r="XW17" s="25"/>
+      <c r="XX17" s="25"/>
+      <c r="XY17" s="25"/>
+      <c r="XZ17" s="25"/>
+      <c r="YA17" s="25"/>
+      <c r="YB17" s="25"/>
+      <c r="YC17" s="25"/>
+      <c r="YD17" s="25"/>
+      <c r="YE17" s="25"/>
+      <c r="YF17" s="25"/>
+      <c r="YG17" s="25"/>
+      <c r="YH17" s="25"/>
+      <c r="YI17" s="25"/>
+      <c r="YJ17" s="25"/>
+      <c r="YK17" s="25"/>
+      <c r="YL17" s="25"/>
+      <c r="YM17" s="25"/>
+      <c r="YN17" s="25"/>
+      <c r="YO17" s="25"/>
+      <c r="YP17" s="25"/>
+      <c r="YQ17" s="25"/>
+      <c r="YR17" s="25"/>
+      <c r="YS17" s="25"/>
+      <c r="YT17" s="25"/>
+      <c r="YU17" s="25"/>
+      <c r="YV17" s="25"/>
+      <c r="YW17" s="25"/>
+      <c r="YX17" s="25"/>
+      <c r="YY17" s="25"/>
+      <c r="YZ17" s="25"/>
+      <c r="ZA17" s="25"/>
+      <c r="ZB17" s="25"/>
+      <c r="ZC17" s="25"/>
+      <c r="ZD17" s="25"/>
+      <c r="ZE17" s="25"/>
+      <c r="ZF17" s="25"/>
+      <c r="ZG17" s="25"/>
+      <c r="ZH17" s="25"/>
+      <c r="ZI17" s="25"/>
+      <c r="ZJ17" s="25"/>
+      <c r="ZK17" s="25"/>
+      <c r="ZL17" s="25"/>
+      <c r="ZM17" s="25"/>
+      <c r="ZN17" s="25"/>
+      <c r="ZO17" s="25"/>
+      <c r="ZP17" s="25"/>
+      <c r="ZQ17" s="25"/>
+      <c r="ZR17" s="25"/>
+      <c r="ZS17" s="25"/>
+      <c r="ZT17" s="25"/>
+      <c r="ZU17" s="25"/>
+      <c r="ZV17" s="25"/>
+      <c r="ZW17" s="25"/>
+      <c r="ZX17" s="25"/>
+      <c r="ZY17" s="25"/>
+      <c r="ZZ17" s="25"/>
+      <c r="AAA17" s="25"/>
+      <c r="AAB17" s="25"/>
+      <c r="AAC17" s="25"/>
+      <c r="AAD17" s="25"/>
+      <c r="AAE17" s="25"/>
+      <c r="AAF17" s="25"/>
+      <c r="AAG17" s="25"/>
+      <c r="AAH17" s="25"/>
+      <c r="AAI17" s="25"/>
+      <c r="AAJ17" s="25"/>
+      <c r="AAK17" s="25"/>
+      <c r="AAL17" s="25"/>
+      <c r="AAM17" s="25"/>
+      <c r="AAN17" s="25"/>
+      <c r="AAO17" s="25"/>
+      <c r="AAP17" s="25"/>
+      <c r="AAQ17" s="25"/>
+      <c r="AAR17" s="25"/>
+      <c r="AAS17" s="25"/>
+      <c r="AAT17" s="25"/>
+      <c r="AAU17" s="25"/>
+      <c r="AAV17" s="25"/>
+      <c r="AAW17" s="25"/>
+      <c r="AAX17" s="25"/>
+      <c r="AAY17" s="25"/>
+      <c r="AAZ17" s="25"/>
+      <c r="ABA17" s="25"/>
+      <c r="ABB17" s="25"/>
+      <c r="ABC17" s="25"/>
+      <c r="ABD17" s="25"/>
+      <c r="ABE17" s="25"/>
+      <c r="ABF17" s="25"/>
+      <c r="ABG17" s="25"/>
+      <c r="ABH17" s="25"/>
+      <c r="ABI17" s="25"/>
+      <c r="ABJ17" s="25"/>
+      <c r="ABK17" s="25"/>
+      <c r="ABL17" s="25"/>
+      <c r="ABM17" s="25"/>
+      <c r="ABN17" s="25"/>
+      <c r="ABO17" s="25"/>
+      <c r="ABP17" s="25"/>
+      <c r="ABQ17" s="25"/>
+      <c r="ABR17" s="25"/>
+      <c r="ABS17" s="25"/>
+      <c r="ABT17" s="25"/>
+      <c r="ABU17" s="25"/>
+      <c r="ABV17" s="25"/>
+      <c r="ABW17" s="25"/>
+      <c r="ABX17" s="25"/>
+      <c r="ABY17" s="25"/>
+      <c r="ABZ17" s="25"/>
+      <c r="ACA17" s="25"/>
+      <c r="ACB17" s="25"/>
+      <c r="ACC17" s="25"/>
+      <c r="ACD17" s="25"/>
+      <c r="ACE17" s="25"/>
+      <c r="ACF17" s="25"/>
+      <c r="ACG17" s="25"/>
+      <c r="ACH17" s="25"/>
+      <c r="ACI17" s="25"/>
+      <c r="ACJ17" s="25"/>
+      <c r="ACK17" s="25"/>
+      <c r="ACL17" s="25"/>
+      <c r="ACM17" s="25"/>
+      <c r="ACN17" s="25"/>
+      <c r="ACO17" s="25"/>
+      <c r="ACP17" s="25"/>
+      <c r="ACQ17" s="25"/>
+      <c r="ACR17" s="25"/>
+      <c r="ACS17" s="25"/>
+      <c r="ACT17" s="25"/>
+      <c r="ACU17" s="25"/>
+      <c r="ACV17" s="25"/>
+      <c r="ACW17" s="25"/>
+      <c r="ACX17" s="25"/>
+      <c r="ACY17" s="25"/>
+      <c r="ACZ17" s="25"/>
+      <c r="ADA17" s="25"/>
+      <c r="ADB17" s="25"/>
+      <c r="ADC17" s="25"/>
+      <c r="ADD17" s="25"/>
+      <c r="ADE17" s="25"/>
+      <c r="ADF17" s="25"/>
+      <c r="ADG17" s="25"/>
+      <c r="ADH17" s="25"/>
+      <c r="ADI17" s="25"/>
+      <c r="ADJ17" s="25"/>
+      <c r="ADK17" s="25"/>
+      <c r="ADL17" s="25"/>
+      <c r="ADM17" s="25"/>
+      <c r="ADN17" s="25"/>
+      <c r="ADO17" s="25"/>
+      <c r="ADP17" s="25"/>
+      <c r="ADQ17" s="25"/>
+      <c r="ADR17" s="25"/>
+      <c r="ADS17" s="25"/>
+      <c r="ADT17" s="25"/>
+      <c r="ADU17" s="25"/>
+      <c r="ADV17" s="25"/>
+      <c r="ADW17" s="25"/>
+      <c r="ADX17" s="25"/>
+      <c r="ADY17" s="25"/>
+      <c r="ADZ17" s="25"/>
+      <c r="AEA17" s="25"/>
+      <c r="AEB17" s="25"/>
+      <c r="AEC17" s="25"/>
+      <c r="AED17" s="25"/>
+      <c r="AEE17" s="25"/>
+      <c r="AEF17" s="25"/>
+      <c r="AEG17" s="25"/>
+      <c r="AEH17" s="25"/>
+      <c r="AEI17" s="25"/>
+      <c r="AEJ17" s="25"/>
+      <c r="AEK17" s="25"/>
+      <c r="AEL17" s="25"/>
+      <c r="AEM17" s="25"/>
+      <c r="AEN17" s="25"/>
+      <c r="AEO17" s="25"/>
+      <c r="AEP17" s="25"/>
+      <c r="AEQ17" s="25"/>
+      <c r="AER17" s="25"/>
+      <c r="AES17" s="25"/>
+      <c r="AET17" s="25"/>
+      <c r="AEU17" s="25"/>
+      <c r="AEV17" s="25"/>
+      <c r="AEW17" s="25"/>
+      <c r="AEX17" s="25"/>
+      <c r="AEY17" s="25"/>
+      <c r="AEZ17" s="25"/>
+      <c r="AFA17" s="25"/>
+      <c r="AFB17" s="25"/>
+      <c r="AFC17" s="25"/>
+      <c r="AFD17" s="25"/>
+      <c r="AFE17" s="25"/>
+      <c r="AFF17" s="25"/>
+      <c r="AFG17" s="25"/>
+      <c r="AFH17" s="25"/>
+      <c r="AFI17" s="25"/>
+      <c r="AFJ17" s="25"/>
+      <c r="AFK17" s="25"/>
+      <c r="AFL17" s="25"/>
+      <c r="AFM17" s="25"/>
+      <c r="AFN17" s="25"/>
+      <c r="AFO17" s="25"/>
+      <c r="AFP17" s="25"/>
+      <c r="AFQ17" s="25"/>
+      <c r="AFR17" s="25"/>
+      <c r="AFS17" s="25"/>
+      <c r="AFT17" s="25"/>
+      <c r="AFU17" s="25"/>
+      <c r="AFV17" s="25"/>
+      <c r="AFW17" s="25"/>
+      <c r="AFX17" s="25"/>
+      <c r="AFY17" s="25"/>
+      <c r="AFZ17" s="25"/>
+      <c r="AGA17" s="25"/>
+      <c r="AGB17" s="25"/>
+      <c r="AGC17" s="25"/>
+      <c r="AGD17" s="25"/>
+      <c r="AGE17" s="25"/>
+      <c r="AGF17" s="25"/>
+      <c r="AGG17" s="25"/>
+      <c r="AGH17" s="25"/>
+      <c r="AGI17" s="25"/>
+      <c r="AGJ17" s="25"/>
+      <c r="AGK17" s="25"/>
+      <c r="AGL17" s="25"/>
+      <c r="AGM17" s="25"/>
+      <c r="AGN17" s="25"/>
+      <c r="AGO17" s="25"/>
+      <c r="AGP17" s="25"/>
+      <c r="AGQ17" s="25"/>
+      <c r="AGR17" s="25"/>
+      <c r="AGS17" s="25"/>
+      <c r="AGT17" s="25"/>
+      <c r="AGU17" s="25"/>
+      <c r="AGV17" s="25"/>
+      <c r="AGW17" s="25"/>
+      <c r="AGX17" s="25"/>
+      <c r="AGY17" s="25"/>
+      <c r="AGZ17" s="25"/>
+      <c r="AHA17" s="25"/>
+      <c r="AHB17" s="25"/>
+      <c r="AHC17" s="25"/>
+      <c r="AHD17" s="25"/>
+      <c r="AHE17" s="25"/>
+      <c r="AHF17" s="25"/>
+      <c r="AHG17" s="25"/>
+      <c r="AHH17" s="25"/>
+      <c r="AHI17" s="25"/>
+      <c r="AHJ17" s="25"/>
+      <c r="AHK17" s="25"/>
+      <c r="AHL17" s="25"/>
+      <c r="AHM17" s="25"/>
+      <c r="AHN17" s="25"/>
+      <c r="AHO17" s="25"/>
+      <c r="AHP17" s="25"/>
+      <c r="AHQ17" s="25"/>
+      <c r="AHR17" s="25"/>
+      <c r="AHS17" s="25"/>
+      <c r="AHT17" s="25"/>
+      <c r="AHU17" s="25"/>
+      <c r="AHV17" s="25"/>
+      <c r="AHW17" s="25"/>
+      <c r="AHX17" s="25"/>
+      <c r="AHY17" s="25"/>
+      <c r="AHZ17" s="25"/>
+      <c r="AIA17" s="25"/>
+      <c r="AIB17" s="25"/>
+      <c r="AIC17" s="25"/>
+      <c r="AID17" s="25"/>
+      <c r="AIE17" s="25"/>
+      <c r="AIF17" s="25"/>
+      <c r="AIG17" s="25"/>
+      <c r="AIH17" s="25"/>
+      <c r="AII17" s="25"/>
+      <c r="AIJ17" s="25"/>
+      <c r="AIK17" s="25"/>
+      <c r="AIL17" s="25"/>
+      <c r="AIM17" s="25"/>
+      <c r="AIN17" s="25"/>
+      <c r="AIO17" s="25"/>
+      <c r="AIP17" s="25"/>
+      <c r="AIQ17" s="25"/>
+      <c r="AIR17" s="25"/>
+      <c r="AIS17" s="25"/>
+      <c r="AIT17" s="25"/>
+      <c r="AIU17" s="25"/>
+      <c r="AIV17" s="25"/>
+      <c r="AIW17" s="25"/>
+      <c r="AIX17" s="25"/>
+      <c r="AIY17" s="25"/>
+      <c r="AIZ17" s="25"/>
+      <c r="AJA17" s="25"/>
+      <c r="AJB17" s="25"/>
+      <c r="AJC17" s="25"/>
+      <c r="AJD17" s="25"/>
+      <c r="AJE17" s="25"/>
+      <c r="AJF17" s="25"/>
+      <c r="AJG17" s="25"/>
+      <c r="AJH17" s="25"/>
+      <c r="AJI17" s="25"/>
+      <c r="AJJ17" s="25"/>
+      <c r="AJK17" s="25"/>
+      <c r="AJL17" s="25"/>
+      <c r="AJM17" s="25"/>
+      <c r="AJN17" s="25"/>
+      <c r="AJO17" s="25"/>
+      <c r="AJP17" s="25"/>
+      <c r="AJQ17" s="25"/>
+      <c r="AJR17" s="25"/>
+      <c r="AJS17" s="25"/>
+      <c r="AJT17" s="25"/>
+      <c r="AJU17" s="25"/>
+      <c r="AJV17" s="25"/>
+      <c r="AJW17" s="25"/>
+      <c r="AJX17" s="25"/>
+      <c r="AJY17" s="25"/>
+      <c r="AJZ17" s="25"/>
+      <c r="AKA17" s="25"/>
+      <c r="AKB17" s="25"/>
+      <c r="AKC17" s="25"/>
+      <c r="AKD17" s="25"/>
+      <c r="AKE17" s="25"/>
+      <c r="AKF17" s="25"/>
+      <c r="AKG17" s="25"/>
+      <c r="AKH17" s="25"/>
+      <c r="AKI17" s="25"/>
+      <c r="AKJ17" s="25"/>
+      <c r="AKK17" s="25"/>
+      <c r="AKL17" s="25"/>
+      <c r="AKM17" s="25"/>
+      <c r="AKN17" s="25"/>
+      <c r="AKO17" s="25"/>
+      <c r="AKP17" s="25"/>
+      <c r="AKQ17" s="25"/>
+      <c r="AKR17" s="25"/>
+      <c r="AKS17" s="25"/>
+      <c r="AKT17" s="25"/>
+      <c r="AKU17" s="25"/>
+      <c r="AKV17" s="25"/>
+      <c r="AKW17" s="25"/>
+      <c r="AKX17" s="25"/>
+      <c r="AKY17" s="25"/>
+      <c r="AKZ17" s="25"/>
+      <c r="ALA17" s="25"/>
+      <c r="ALB17" s="25"/>
+      <c r="ALC17" s="25"/>
+      <c r="ALD17" s="25"/>
+      <c r="ALE17" s="25"/>
+      <c r="ALF17" s="25"/>
+      <c r="ALG17" s="25"/>
+      <c r="ALH17" s="25"/>
+      <c r="ALI17" s="25"/>
+      <c r="ALJ17" s="25"/>
+      <c r="ALK17" s="25"/>
+      <c r="ALL17" s="25"/>
+      <c r="ALM17" s="25"/>
+      <c r="ALN17" s="25"/>
+      <c r="ALO17" s="25"/>
+      <c r="ALP17" s="25"/>
+      <c r="ALQ17" s="25"/>
+      <c r="ALR17" s="25"/>
+      <c r="ALS17" s="25"/>
+      <c r="ALT17" s="25"/>
+      <c r="ALU17" s="25"/>
+      <c r="ALV17" s="25"/>
+      <c r="ALW17" s="25"/>
+      <c r="ALX17" s="25"/>
+      <c r="ALY17" s="25"/>
+      <c r="ALZ17" s="25"/>
+      <c r="AMA17" s="25"/>
+      <c r="AMB17" s="25"/>
+      <c r="AMC17" s="25"/>
+      <c r="AMD17" s="25"/>
+      <c r="AME17" s="25"/>
+      <c r="AMF17" s="25"/>
+      <c r="AMG17" s="25"/>
+      <c r="AMH17" s="25"/>
+      <c r="AMI17" s="25"/>
+      <c r="AMJ17" s="25"/>
+      <c r="AMK17" s="25"/>
+    </row>
+    <row r="24" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="M24" s="13" t="s">
         <v>5</v>
       </c>
@@ -5027,7 +7522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="M25" s="16">
         <f>SUM(F:F)</f>
         <v>1300</v>
@@ -5053,7 +7548,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5251,7 +7746,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K24"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5389,7 +7884,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K14"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,7 +8105,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>